<commit_message>
Update SLA-1500-FFC_RevC_Bill of Materials.xlsx
</commit_message>
<xml_diff>
--- a/Docs/Schematics/SLA-1500-FFC_RevC_Bill of Materials.xlsx
+++ b/Docs/Schematics/SLA-1500-FFC_RevC_Bill of Materials.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/447eb0fe645bf98e/Documents/GitHub/Capstone-Sightline/Docs/Schematics/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phamt\Documents\GitHub\Capstone-Sightline\Docs\Schematics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_12B1CC87528EB491CBCB8711A2B3E7908CBCC35A" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{B72A804C-9058-4174-9D99-8475CA357A7D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF74C414-8CCE-4705-81D3-53E3A85DEEFB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7485" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -991,7 +990,7 @@
   <dimension ref="A1:G1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>